<commit_message>
Fixed NYC data clean (#7)
* Corrected NYC cleanup in c_d_withstate_df

* NYC cleanup after saving the file
</commit_message>
<xml_diff>
--- a/data_manipulation/source_data/naming_review.xlsx
+++ b/data_manipulation/source_data/naming_review.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlund\Documents\GitHub\project_one\data_manipulation\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47F88AD2-1095-44F4-A326-7D0F6F7A00D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CACC75-3333-427D-AC43-487964F2141F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{7FF4B16E-6BC2-4EC2-8316-7A5D47F6A7F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22260" windowHeight="13176" xr2:uid="{7FF4B16E-6BC2-4EC2-8316-7A5D47F6A7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$P$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$A$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="147">
   <si>
     <t>Vaccine Allocation</t>
   </si>
@@ -465,7 +467,10 @@
     <t>State_codes</t>
   </si>
   <si>
-    <t>GV</t>
+    <t>Corrected before merge</t>
+  </si>
+  <si>
+    <t>Corrected after merge</t>
   </si>
 </sst>
 </file>
@@ -562,12 +567,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
@@ -575,7 +579,16 @@
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -885,11 +898,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3AE7F8-F472-462E-970D-F123738418F3}">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -899,9 +912,10 @@
     <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>144</v>
       </c>
@@ -918,7 +932,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>140</v>
       </c>
@@ -935,7 +949,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -952,7 +966,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -968,8 +982,11 @@
       <c r="E4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G4" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -985,8 +1002,11 @@
       <c r="E5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G5" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1003,7 +1023,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1020,7 +1040,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1037,7 +1057,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1054,7 +1074,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1071,7 +1091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1088,7 +1108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1105,7 +1125,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1122,7 +1142,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1139,7 +1159,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1156,7 +1176,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -1208,7 +1228,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1570,10 +1590,10 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1714,7 +1734,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1956,72 +1976,36 @@
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
+    <row r="65" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E65" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E66" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
+    </row>
+    <row r="67" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E67" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
+    </row>
+    <row r="68" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E68" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B68" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E69" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B69" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
+    </row>
+    <row r="70" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D70" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B70" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E70" s="3" t="s">
+      <c r="E70" s="4" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2033,4 +2017,336 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2AEFA1E-869F-41F9-A02A-03621AC9C225}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:A61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K71" sqref="K71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A61" xr:uid="{A3CACE43-F848-4C77-9D11-62328EC9C987}">
+    <filterColumn colId="0">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A27121">
+    <sortCondition ref="A2:A27121"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>